<commit_message>
Loans can now be settled
</commit_message>
<xml_diff>
--- a/Database/BrokerBasics.xlsx
+++ b/Database/BrokerBasics.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,24 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -330,13 +317,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col customWidth="1" max="9" min="1" width="30"/>
+    <col customWidth="1" max="2" min="2" width="30"/>
+    <col customWidth="1" max="3" min="3" width="30"/>
+    <col customWidth="1" max="4" min="4" width="30"/>
+    <col customWidth="1" max="5" min="5" width="30"/>
+    <col customWidth="1" max="6" min="6" width="30"/>
+    <col customWidth="1" max="7" min="7" width="30"/>
+    <col customWidth="1" max="8" min="8" width="30"/>
+    <col customWidth="1" max="9" min="9" width="30"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Broker Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Amount In Hand</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>No. of Customers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Settled Customers</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Total Customers</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Loan Given</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Loan Settled</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Loan till date</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Broker Address</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>divesh</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9979578</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20422</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20422</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>muthu street</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>nilesh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>120000</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>muthu street</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Broker file is updated when file settled although constraints yet to be added
</commit_message>
<xml_diff>
--- a/Database/BrokerBasics.xlsx
+++ b/Database/BrokerBasics.xlsx
@@ -388,7 +388,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -428,28 +427,26 @@
           <t>nilesh</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>120000</t>
-        </is>
+      <c r="B4" t="n">
+        <v>138000</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
File option works completely
</commit_message>
<xml_diff>
--- a/Database/BrokerBasics.xlsx
+++ b/Database/BrokerBasics.xlsx
@@ -395,25 +395,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9979578</v>
+        <v>9968578</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>20422</v>
+        <v>32422</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>20422</v>
+        <v>32422</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Editing the Loan amount feature added
</commit_message>
<xml_diff>
--- a/Database/BrokerBasics.xlsx
+++ b/Database/BrokerBasics.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -322,23 +322,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col customWidth="1" max="9" min="1" width="30"/>
-    <col customWidth="1" max="2" min="2" width="30"/>
-    <col customWidth="1" max="3" min="3" width="30"/>
-    <col customWidth="1" max="4" min="4" width="30"/>
-    <col customWidth="1" max="5" min="5" width="30"/>
-    <col customWidth="1" max="6" min="6" width="30"/>
-    <col customWidth="1" max="7" min="7" width="30"/>
-    <col customWidth="1" max="8" min="8" width="30"/>
-    <col customWidth="1" max="9" min="9" width="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -388,6 +380,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -395,25 +388,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9968578</v>
+        <v>9864121</v>
       </c>
       <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
         <v>3</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>32422</v>
+        <v>229965</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="H3" t="n">
-        <v>32422</v>
+        <v>229965</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -451,6 +444,111 @@
       <c r="I4" t="inlineStr">
         <is>
           <t>muthu street</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>navjyoti</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1200000</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Jatin</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1000000</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>xyz colony</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mangal</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2000000</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>l-427</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Broker Files can now be modified
</commit_message>
<xml_diff>
--- a/Database/BrokerBasics.xlsx
+++ b/Database/BrokerBasics.xlsx
@@ -384,11 +384,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>divesh</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>9864121</v>
+          <t>divesh_jain</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1234567</t>
+        </is>
       </c>
       <c r="C3" t="n">
         <v>8</v>
@@ -410,7 +412,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>muthu street</t>
+          <t>vaichur muthiah street</t>
         </is>
       </c>
     </row>

</xml_diff>